<commit_message>
agrego etiquetas de Noviembre 2021
</commit_message>
<xml_diff>
--- a/Etiquetas/Nov2021/EtiquetasTortugometroNoviembre2021_T185_hembra.xlsx
+++ b/Etiquetas/Nov2021/EtiquetasTortugometroNoviembre2021_T185_hembra.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modulos resumen" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="103">
   <si>
     <t xml:space="preserve">ejemplar</t>
   </si>
@@ -216,6 +216,9 @@
     <t xml:space="preserve">sigue en refugio quieta</t>
   </si>
   <si>
+    <t xml:space="preserve">nosabemos</t>
+  </si>
+  <si>
     <t xml:space="preserve">no estaba mas en refugio camino y se acabo el hilo, 12:42 relevamiento hilo GPS de Fer inicio 138-199-330 final del hilo.</t>
   </si>
   <si>
@@ -226,6 +229,15 @@
   </si>
   <si>
     <t xml:space="preserve">la encontramos en otro refugio comiendo bajo coirones, colocamos hilo nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copulando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copulando con macho erguido a 4 grados sobre la hembra 185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continua la copula</t>
   </si>
   <si>
     <t xml:space="preserve">bajo coiron con T76 IMU prendido</t>
@@ -333,7 +345,7 @@
     <numFmt numFmtId="168" formatCode="h:mm:ss"/>
     <numFmt numFmtId="169" formatCode="m/d/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -361,12 +373,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -466,7 +472,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,11 +556,11 @@
   </sheetPr>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.09"/>
   </cols>
@@ -915,13 +921,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.32"/>
@@ -1066,6 +1072,9 @@
       <c r="H8" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="I8" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="K8" s="0" t="s">
         <v>40</v>
       </c>
@@ -1363,9 +1372,12 @@
       <c r="G25" s="2" t="n">
         <v>44525</v>
       </c>
+      <c r="H25" s="0" t="s">
+        <v>64</v>
+      </c>
       <c r="J25" s="10"/>
       <c r="K25" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,19 +1388,19 @@
         <v>0.553472222222222</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G26" s="2" t="n">
         <v>44525</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I26" s="0" t="s">
         <v>31</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,37 +1408,50 @@
         <v>9</v>
       </c>
       <c r="B27" s="6" t="n">
-        <v>0.888194444444444</v>
+        <v>0.559027777777778</v>
       </c>
       <c r="G27" s="2" t="n">
         <v>44525</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3"/>
-      <c r="G28" s="2"/>
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>0.565972222222222</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>44525</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="11" t="n">
-        <v>0.305555555555556</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>69</v>
+      <c r="B29" s="6" t="n">
+        <v>0.888194444444444</v>
       </c>
       <c r="G29" s="2" t="n">
-        <v>44526</v>
+        <v>44525</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>39</v>
@@ -1435,47 +1460,34 @@
         <v>35</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="11" t="n">
-        <v>0.382638888888889</v>
-      </c>
-      <c r="G30" s="2" t="n">
-        <v>44526</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>71</v>
-      </c>
+      <c r="B30" s="3"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B31" s="11" t="n">
-        <v>0.397916666666667</v>
+        <v>0.305555555555556</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="G31" s="2" t="n">
         <v>44526</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,19 +1495,19 @@
         <v>9</v>
       </c>
       <c r="B32" s="11" t="n">
-        <v>0.403472222222222</v>
+        <v>0.382638888888889</v>
       </c>
       <c r="G32" s="2" t="n">
         <v>44526</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,19 +1515,19 @@
         <v>9</v>
       </c>
       <c r="B33" s="11" t="n">
-        <v>0.436111111111111</v>
+        <v>0.397916666666667</v>
       </c>
       <c r="G33" s="2" t="n">
         <v>44526</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,66 +1535,98 @@
         <v>9</v>
       </c>
       <c r="B34" s="11" t="n">
-        <v>0.527083333333333</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>75</v>
+        <v>0.403472222222222</v>
       </c>
       <c r="G34" s="2" t="n">
         <v>44526</v>
       </c>
+      <c r="H34" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="K34" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3"/>
-      <c r="G35" s="2"/>
+      <c r="A35" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>0.436111111111111</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="11" t="n">
+        <v>0.527083333333333</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="11" t="n">
         <v>0.331944444444444</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G38" s="2" t="n">
         <v>44527</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="H38" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="I38" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="11" t="n">
+      <c r="K38" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="11" t="n">
         <v>0.334722222222222</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G39" s="2" t="n">
         <v>44527</v>
       </c>
-      <c r="K37" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="11"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3"/>
-      <c r="G39" s="2"/>
+      <c r="K39" s="0" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3"/>
+      <c r="B40" s="11"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,388 +1653,396 @@
       <c r="B46" s="3"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="3" t="n">
-        <v>0.386111111111111</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" s="0" t="n">
-        <v>-40.5823</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>-65.00053</v>
-      </c>
-      <c r="F52" s="0" t="n">
-        <v>153</v>
-      </c>
-      <c r="G52" s="2" t="n">
-        <v>44582</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B53" s="3" t="n">
-        <v>0.810416666666667</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>-40.58271</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>-65.00127</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>155</v>
-      </c>
-      <c r="G53" s="2" t="n">
-        <v>44582</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I53" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J53" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K53" s="0" t="s">
-        <v>86</v>
-      </c>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3"/>
+      <c r="G48" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B54" s="3" t="n">
-        <v>0.440972222222222</v>
+        <v>0.386111111111111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>-40.5823</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>-65.00053</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>153</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>44583</v>
-      </c>
-      <c r="I54" s="0" t="s">
-        <v>31</v>
+        <v>44582</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B55" s="3" t="n">
-        <v>0.798611111111111</v>
+        <v>0.810416666666667</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>87</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>-40.58305</v>
+        <v>-40.58271</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>-65.00117</v>
+        <v>-65.00127</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G55" s="2" t="n">
-        <v>44583</v>
+        <v>44582</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="L55" s="0" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="M55" s="0" t="n">
-        <v>19.2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B56" s="3" t="n">
-        <v>0.370833333333333</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>-40.58306</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>-65.00117</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>155</v>
+        <v>0.440972222222222</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>44584</v>
-      </c>
-      <c r="H56" s="0" t="s">
-        <v>84</v>
+        <v>44583</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J56" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K56" s="0" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B57" s="3" t="n">
-        <v>0.844444444444444</v>
+        <v>0.798611111111111</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>-40.58479</v>
+        <v>-40.58305</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>-65.00284</v>
+        <v>-65.00117</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G57" s="2" t="n">
-        <v>44584</v>
+        <v>44583</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I57" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>19.2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B58" s="3" t="n">
-        <v>0.354166666666667</v>
+        <v>0.370833333333333</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>-40.58479</v>
+        <v>-40.58306</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>-65.00284</v>
+        <v>-65.00117</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G58" s="2" t="n">
-        <v>44585</v>
+        <v>44584</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I58" s="0" t="s">
         <v>35</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B59" s="3" t="n">
-        <v>0.4375</v>
+        <v>0.844444444444444</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>-40.58475</v>
+        <v>-40.58479</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>-65.00166</v>
+        <v>-65.00284</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G59" s="2" t="n">
-        <v>44586</v>
+        <v>44584</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="K59" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="3" t="n">
+        <v>0.354166666666667</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="L59" s="0" t="n">
-        <v>39.5</v>
-      </c>
-      <c r="M59" s="0" t="n">
-        <v>21.1</v>
+      <c r="D60" s="0" t="n">
+        <v>-40.58479</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>-65.00284</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="G60" s="2" t="n">
+        <v>44585</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B61" s="3" t="n">
-        <v>0.498611111111111</v>
+        <v>0.4375</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>-40.58435</v>
+        <v>-40.58475</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>-64.9971</v>
+        <v>-65.00166</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G61" s="2" t="n">
-        <v>44582</v>
+        <v>44586</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B62" s="3" t="n">
-        <v>0.873611111111111</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="D62" s="0" t="n">
-        <v>-40.58412</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <v>-64.99645</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>152</v>
-      </c>
-      <c r="G62" s="2" t="n">
-        <v>44582</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="K62" s="0" t="s">
         <v>97</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <v>21.1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B63" s="3" t="n">
-        <v>0.413194444444444</v>
+        <v>0.498611111111111</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>-40.58353</v>
+        <v>-40.58435</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>-64.99465</v>
+        <v>-64.9971</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G63" s="2" t="n">
-        <v>44584</v>
+        <v>44582</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="I63" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J63" s="0" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B64" s="3" t="n">
+        <v>0.873611111111111</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>-40.58412</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>-64.99645</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>152</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>44582</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="3" t="n">
+        <v>0.413194444444444</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>-40.58353</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>-64.99465</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="G65" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="3" t="n">
         <v>0.395833333333333</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D66" s="0" t="n">
         <v>-40.58533</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E66" s="0" t="n">
         <v>-64.99138</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F66" s="0" t="n">
         <v>147</v>
       </c>
-      <c r="G64" s="2" t="n">
+      <c r="G66" s="2" t="n">
         <v>44586</v>
       </c>
-      <c r="H64" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="I64" s="0" t="s">
+      <c r="H66" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I66" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J64" s="0" t="s">
+      <c r="J66" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K64" s="0" t="s">
-        <v>98</v>
+      <c r="K66" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +2067,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>